<commit_message>
Adds country stats chart
</commit_message>
<xml_diff>
--- a/gbif-ipt-docs/stats/IPT-Stats.xlsx
+++ b/gbif-ipt-docs/stats/IPT-Stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="420" windowWidth="33160" windowHeight="21920" tabRatio="500"/>
+    <workbookView xWindow="3240" yWindow="420" windowWidth="25560" windowHeight="21800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
   <si>
     <t># Metadata-only datasets published by IPTs</t>
   </si>
@@ -137,8 +137,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -214,7 +216,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -247,6 +249,7 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -279,6 +282,7 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -433,11 +437,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2113217064"/>
-        <c:axId val="-2112720936"/>
+        <c:axId val="2117890392"/>
+        <c:axId val="2117893528"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2113217064"/>
+        <c:axId val="2117890392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -447,7 +451,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112720936"/>
+        <c:crossAx val="2117893528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -456,7 +460,7 @@
         <c:majorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2112720936"/>
+        <c:axId val="2117893528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0E8"/>
@@ -468,7 +472,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113217064"/>
+        <c:crossAx val="2117890392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -649,11 +653,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2112901736"/>
-        <c:axId val="2115383608"/>
+        <c:axId val="2117965976"/>
+        <c:axId val="2117968616"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2112901736"/>
+        <c:axId val="2117965976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -663,7 +667,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115383608"/>
+        <c:crossAx val="2117968616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -672,7 +676,7 @@
         <c:majorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2115383608"/>
+        <c:axId val="2117968616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="80.0"/>
@@ -684,7 +688,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112901736"/>
+        <c:crossAx val="2117965976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1223,11 +1227,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2113412792"/>
-        <c:axId val="2115629592"/>
+        <c:axId val="2118031912"/>
+        <c:axId val="2118034968"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2113412792"/>
+        <c:axId val="2118031912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,7 +1241,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115629592"/>
+        <c:crossAx val="2118034968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -1246,7 +1250,7 @@
         <c:majorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2115629592"/>
+        <c:axId val="2118034968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-30.0"/>
@@ -1258,7 +1262,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113412792"/>
+        <c:crossAx val="2118031912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1750,11 +1754,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2124176760"/>
-        <c:axId val="2123411384"/>
+        <c:axId val="2118086728"/>
+        <c:axId val="2118089784"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2124176760"/>
+        <c:axId val="2118086728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1764,7 +1768,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123411384"/>
+        <c:crossAx val="2118089784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1775,7 +1779,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2123411384"/>
+        <c:axId val="2118089784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1786,7 +1790,234 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124176760"/>
+        <c:crossAx val="2118086728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="0"/>
+      </c:dTable>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t># Countries IPTs are installed in</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.273568926394161"/>
+          <c:y val="0.0221674876847291"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># Countries IPTs are installed in</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$1:$J$1</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>41730.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42064.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42248.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42293.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42705.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42795.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42998.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43073.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$J$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="r"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2117261256"/>
+        <c:axId val="2117258648"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="2117261256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2117258648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+        <c:majorUnit val="1.0"/>
+        <c:majorTimeUnit val="years"/>
+        <c:minorUnit val="1.0"/>
+        <c:minorTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="2117258648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="65.0"/>
+          <c:min val="35.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="2117261256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1931,6 +2162,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>195</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2263,8 +2526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2349,8 +2612,8 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>87</v>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
       <c r="C3">
         <v>42</v>

</xml_diff>